<commit_message>
excelReader returns a collection of data
</commit_message>
<xml_diff>
--- a/IceElemental/ExcelReports/Furniture2007.xlsx
+++ b/IceElemental/ExcelReports/Furniture2007.xlsx
@@ -361,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="B1" sqref="B1"/>
@@ -413,6 +413,42 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
override the excel table
</commit_message>
<xml_diff>
--- a/IceElemental/ExcelReports/Furniture2007.xlsx
+++ b/IceElemental/ExcelReports/Furniture2007.xlsx
@@ -361,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="B1" sqref="B1"/>
@@ -449,6 +449,30 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
json parser, mysql dbcontext and some other things
</commit_message>
<xml_diff>
--- a/IceElemental/ExcelReports/Furniture2007.xlsx
+++ b/IceElemental/ExcelReports/Furniture2007.xlsx
@@ -361,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="B1" sqref="B1"/>
@@ -485,6 +485,66 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>Videnov</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>Sofia, Tsarigradsko, 15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>